<commit_message>
changes to excel sheets
</commit_message>
<xml_diff>
--- a/answer-key.xlsx
+++ b/answer-key.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\R\Projects\thrones-pool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D866CE1F-9B68-4AA5-8A43-E72442DBD6A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39CC7702-679C-4C97-9E84-497B5AA40D16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -261,7 +261,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -466,21 +466,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="15"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="15"/>
       </left>
       <right style="thin">
@@ -491,21 +476,6 @@
       </top>
       <bottom style="thin">
         <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -561,13 +531,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -604,12 +587,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -619,12 +602,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -640,13 +617,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1815,7 +1804,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
@@ -1849,14 +1838,14 @@
     </row>
     <row r="3" spans="1:7" ht="24.2" customHeight="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
+      <c r="B3" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
     </row>
     <row r="4" spans="1:7" ht="21.4" customHeight="1">
       <c r="A4" s="4"/>
@@ -2301,68 +2290,68 @@
     </row>
     <row r="25" spans="1:7" ht="24.6" customHeight="1">
       <c r="A25" s="4"/>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
       <c r="E25" s="16"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="23"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="21"/>
     </row>
     <row r="26" spans="1:7" ht="20.65" customHeight="1">
       <c r="A26" s="4"/>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="18"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="24"/>
       <c r="G26" s="11"/>
     </row>
     <row r="27" spans="1:7" ht="20.65" customHeight="1">
       <c r="A27" s="4"/>
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="27"/>
       <c r="G27" s="11"/>
     </row>
     <row r="28" spans="1:7" ht="20.65" customHeight="1">
       <c r="A28" s="4"/>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="18"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="24"/>
       <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:7" ht="20.65" customHeight="1">
       <c r="A29" s="4"/>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="18"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="24"/>
       <c r="G29" s="11"/>
     </row>
     <row r="30" spans="1:7" ht="20.65" customHeight="1">
       <c r="A30" s="4"/>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="18"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="24"/>
       <c r="G30" s="12"/>
     </row>
     <row r="31" spans="1:7" ht="32.65" customHeight="1">
@@ -2370,10 +2359,10 @@
       <c r="B31" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="17"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="13"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed format of excel file
</commit_message>
<xml_diff>
--- a/answer-key.xlsx
+++ b/answer-key.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\R\Projects\thrones-pool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tylerbradley/Documents/thrones-pool/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39CC7702-679C-4C97-9E84-497B5AA40D16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC65A19-17D9-4647-9EC3-03E66FAF7466}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15960" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
   <si>
     <t>Table 1</t>
   </si>
@@ -160,18 +160,6 @@
     <t>Bonus Questions</t>
   </si>
   <si>
-    <t>Who kills the Night King?…if killed (3)</t>
-  </si>
-  <si>
-    <t>Who kills Cercei? … if killed (3)</t>
-  </si>
-  <si>
-    <t>Who dies first? (2pts)</t>
-  </si>
-  <si>
-    <t>Who dies last? (2)</t>
-  </si>
-  <si>
     <t>Name:</t>
   </si>
   <si>
@@ -181,14 +169,47 @@
     <t>Winner of CLEGANEBOWL? (2)</t>
   </si>
   <si>
-    <t>Who wins the Game of Thrones? (5) **If only one person guesses correctly they win 20% of pool and a prize**</t>
+    <t xml:space="preserve">Who dies first? (2pts) </t>
+  </si>
+  <si>
+    <t>Who dies last? (2 pts)</t>
+  </si>
+  <si>
+    <t>Who kills the Night King?…if killed (3) **If you think he lives put “safe” **</t>
+  </si>
+  <si>
+    <t>John Snow</t>
+  </si>
+  <si>
+    <t>Who kills Cercei? … if killed (3) **If you think this bitch lives put “safe” **</t>
+  </si>
+  <si>
+    <t>Will we see an undead Ned Stark? (2) … yes or no answer</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Over / under how many Stark children survive: +1.5 (2)</t>
+  </si>
+  <si>
+    <t>Under</t>
+  </si>
+  <si>
+    <t>Over / under the number of people Arya kills: +3.5 (2)</t>
+  </si>
+  <si>
+    <t>Over</t>
+  </si>
+  <si>
+    <t>Who wins the Game of Thrones??? (5) **If only one person guesses correctly they win 20% of pool and a prize**</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -215,11 +236,6 @@
       <b/>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
@@ -261,7 +277,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -466,21 +482,6 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="15"/>
-      </left>
-      <right style="thin">
-        <color indexed="15"/>
-      </right>
-      <top style="thin">
-        <color indexed="15"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="8"/>
       </left>
       <right style="thin">
@@ -498,12 +499,87 @@
       <left style="thin">
         <color indexed="11"/>
       </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="thin">
+        <color indexed="17"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="17"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
       <right/>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -511,36 +587,53 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="15"/>
+        <color indexed="17"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
       <right style="thin">
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="17"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
       </bottom>
       <diagonal/>
     </border>
@@ -550,7 +643,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -584,58 +677,64 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1798,56 +1897,56 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IV31"/>
+  <dimension ref="A1:IV34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
+      <selection pane="bottomRight" activeCell="B31" sqref="B31:F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="256" width="16.28515625" style="1" customWidth="1"/>
+    <col min="1" max="256" width="16.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.6" customHeight="1">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-    </row>
-    <row r="2" spans="1:7" ht="20.25" customHeight="1">
+    <row r="1" spans="1:7" ht="27.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:7" ht="24.2" customHeight="1">
+    <row r="3" spans="1:7" ht="24.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3"/>
-      <c r="B3" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-    </row>
-    <row r="4" spans="1:7" ht="21.4" customHeight="1">
+      <c r="B3" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+    </row>
+    <row r="4" spans="1:7" ht="21.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
         <v>2</v>
@@ -1868,7 +1967,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="20.65" customHeight="1">
+    <row r="5" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4"/>
       <c r="B5" s="8" t="s">
         <v>5</v>
@@ -1889,7 +1988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="20.65" customHeight="1">
+    <row r="6" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4"/>
       <c r="B6" s="8" t="s">
         <v>7</v>
@@ -1910,7 +2009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="20.65" customHeight="1">
+    <row r="7" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4"/>
       <c r="B7" s="8" t="s">
         <v>9</v>
@@ -1931,7 +2030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="20.65" customHeight="1">
+    <row r="8" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4"/>
       <c r="B8" s="8" t="s">
         <v>11</v>
@@ -1952,7 +2051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="20.65" customHeight="1">
+    <row r="9" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4"/>
       <c r="B9" s="8" t="s">
         <v>13</v>
@@ -1973,7 +2072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="20.65" customHeight="1">
+    <row r="10" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4"/>
       <c r="B10" s="8" t="s">
         <v>15</v>
@@ -1994,7 +2093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="20.65" customHeight="1">
+    <row r="11" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4"/>
       <c r="B11" s="8" t="s">
         <v>17</v>
@@ -2015,7 +2114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="20.65" customHeight="1">
+    <row r="12" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4"/>
       <c r="B12" s="8" t="s">
         <v>19</v>
@@ -2036,7 +2135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="20.65" customHeight="1">
+    <row r="13" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4"/>
       <c r="B13" s="8" t="s">
         <v>21</v>
@@ -2057,7 +2156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="20.65" customHeight="1">
+    <row r="14" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4"/>
       <c r="B14" s="8" t="s">
         <v>23</v>
@@ -2078,7 +2177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="20.65" customHeight="1">
+    <row r="15" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="4"/>
       <c r="B15" s="8" t="s">
         <v>25</v>
@@ -2099,7 +2198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="20.65" customHeight="1">
+    <row r="16" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4"/>
       <c r="B16" s="8" t="s">
         <v>27</v>
@@ -2120,7 +2219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="20.65" customHeight="1">
+    <row r="17" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
       <c r="B17" s="8" t="s">
         <v>29</v>
@@ -2141,7 +2240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="20.65" customHeight="1">
+    <row r="18" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="4"/>
       <c r="B18" s="8" t="s">
         <v>31</v>
@@ -2162,7 +2261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="20.65" customHeight="1">
+    <row r="19" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="4"/>
       <c r="B19" s="8" t="s">
         <v>33</v>
@@ -2183,7 +2282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="20.65" customHeight="1">
+    <row r="20" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="4"/>
       <c r="B20" s="8" t="s">
         <v>35</v>
@@ -2204,7 +2303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="20.65" customHeight="1">
+    <row r="21" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4"/>
       <c r="B21" s="8" t="s">
         <v>37</v>
@@ -2225,7 +2324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="20.65" customHeight="1">
+    <row r="22" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="4"/>
       <c r="B22" s="8" t="s">
         <v>39</v>
@@ -2246,7 +2345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="20.65" customHeight="1">
+    <row r="23" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="4"/>
       <c r="B23" s="8" t="s">
         <v>41</v>
@@ -2267,7 +2366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="20.65" customHeight="1">
+    <row r="24" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="4"/>
       <c r="B24" s="8" t="s">
         <v>43</v>
@@ -2288,85 +2387,139 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="24.6" customHeight="1">
+    <row r="25" spans="1:7" ht="24.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="4"/>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
       <c r="E25" s="16"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="21"/>
-    </row>
-    <row r="26" spans="1:7" ht="20.65" customHeight="1">
-      <c r="A26" s="4"/>
-      <c r="B26" s="25" t="s">
+      <c r="F25" s="15"/>
+      <c r="G25" s="17"/>
+    </row>
+    <row r="26" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="18"/>
+      <c r="B26" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="18"/>
+      <c r="B27" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="18"/>
+      <c r="B28" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="11"/>
-    </row>
-    <row r="27" spans="1:7" ht="20.65" customHeight="1">
-      <c r="A27" s="4"/>
-      <c r="B27" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="11"/>
-    </row>
-    <row r="28" spans="1:7" ht="20.65" customHeight="1">
-      <c r="A28" s="4"/>
-      <c r="B28" s="25" t="s">
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="18"/>
+      <c r="B29" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="11"/>
-    </row>
-    <row r="29" spans="1:7" ht="20.65" customHeight="1">
-      <c r="A29" s="4"/>
-      <c r="B29" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="11"/>
-    </row>
-    <row r="30" spans="1:7" ht="20.65" customHeight="1">
-      <c r="A30" s="4"/>
-      <c r="B30" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="12"/>
-    </row>
-    <row r="31" spans="1:7" ht="32.65" customHeight="1">
-      <c r="A31" s="4"/>
-      <c r="B31" s="15" t="s">
+    </row>
+    <row r="30" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="18"/>
+      <c r="B30" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="13"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="32.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="18"/>
+      <c r="B31" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="18"/>
+      <c r="B32" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="18"/>
+      <c r="B33" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="18"/>
+      <c r="B34" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="30" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="12">
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B31:F31"/>
     <mergeCell ref="B30:F30"/>

</xml_diff>

<commit_message>
added player stats tab and player filter for comparison tab
</commit_message>
<xml_diff>
--- a/answer-key.xlsx
+++ b/answer-key.xlsx
@@ -1,30 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tylerbradley/Documents/thrones-pool/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\R\Projects\thrones-pool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC65A19-17D9-4647-9EC3-03E66FAF7466}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5778308-F8A6-4316-97EE-37B70660FE21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="15960" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="63">
   <si>
     <t>Table 1</t>
   </si>
   <si>
+    <t>Name:</t>
+  </si>
+  <si>
     <t>Game of Thrones Death Pool</t>
   </si>
   <si>
@@ -160,56 +170,99 @@
     <t>Bonus Questions</t>
   </si>
   <si>
-    <t>Name:</t>
-  </si>
-  <si>
-    <t>Master</t>
+    <t xml:space="preserve">Who dies first? (2pts) </t>
+  </si>
+  <si>
+    <t>Who dies last? (2 pts)</t>
   </si>
   <si>
     <t>Winner of CLEGANEBOWL? (2)</t>
   </si>
   <si>
-    <t xml:space="preserve">Who dies first? (2pts) </t>
-  </si>
-  <si>
-    <t>Who dies last? (2 pts)</t>
-  </si>
-  <si>
-    <t>Who kills the Night King?…if killed (3) **If you think he lives put “safe” **</t>
-  </si>
-  <si>
-    <t>John Snow</t>
-  </si>
-  <si>
-    <t>Who kills Cercei? … if killed (3) **If you think this bitch lives put “safe” **</t>
-  </si>
-  <si>
     <t>Will we see an undead Ned Stark? (2) … yes or no answer</t>
   </si>
   <si>
     <t>No</t>
   </si>
   <si>
-    <t>Over / under how many Stark children survive: +1.5 (2)</t>
-  </si>
-  <si>
     <t>Under</t>
   </si>
   <si>
-    <t>Over / under the number of people Arya kills: +3.5 (2)</t>
-  </si>
-  <si>
     <t>Over</t>
   </si>
   <si>
     <t>Who wins the Game of Thrones??? (5) **If only one person guesses correctly they win 20% of pool and a prize**</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Lives/Dies</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>Who kills Cercei? … if killed (3) **If you think this bitch lives pick her name**</t>
+  </si>
+  <si>
+    <t>Who kills the Night King?…if killed (3) **If you think he lives pick his name **</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Over / under how many Stark children survive: +1.5 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Over / under the number of people Arya kills: +3.5 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="0"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (2)</t>
+    </r>
+  </si>
+  <si>
+    <t>Master Key</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -238,8 +291,20 @@
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,13 +325,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
+        <fgColor indexed="14"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="14"/>
+        <fgColor indexed="15"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -276,8 +341,20 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="18"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="25">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -289,9 +366,18 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
-      <right style="thin">
+      <right/>
+      <top style="thin">
         <color indexed="10"/>
-      </right>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color indexed="10"/>
       </top>
@@ -302,7 +388,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
@@ -311,7 +397,7 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -320,190 +406,10 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="15"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="15"/>
-      </left>
-      <right style="thin">
-        <color indexed="15"/>
-      </right>
-      <top style="thin">
-        <color indexed="15"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="15"/>
-      </left>
-      <right style="thin">
-        <color indexed="15"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="15"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="15"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
         <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
         <color indexed="11"/>
@@ -518,7 +424,7 @@
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
         <color indexed="11"/>
@@ -533,7 +439,7 @@
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
         <color indexed="11"/>
@@ -543,6 +449,66 @@
     <border>
       <left style="thin">
         <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="17"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
       </left>
       <right style="thin">
         <color indexed="17"/>
@@ -572,6 +538,21 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="13"/>
       </left>
       <right/>
@@ -598,21 +579,6 @@
       <left/>
       <right style="thin">
         <color indexed="17"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
       </right>
       <top style="thin">
         <color indexed="11"/>
@@ -637,105 +603,167 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top style="thin">
+        <color indexed="17"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="17"/>
+      </left>
+      <right style="thin">
+        <color indexed="17"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="17"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -754,16 +782,16 @@
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFA5A5A5"/>
       <rgbColor rgb="FFBDC0BF"/>
-      <rgbColor rgb="FFA5A5A5"/>
       <rgbColor rgb="FF3F3F3F"/>
       <rgbColor rgb="FFDBDBDB"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FFE8E8E8"/>
       <rgbColor rgb="FF515151"/>
       <rgbColor rgb="FFCCCCCC"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
       <rgbColor rgb="00808000"/>
       <rgbColor rgb="00800080"/>
       <rgbColor rgb="00008080"/>
@@ -833,10 +861,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -1013,11 +1041,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:schemeClr val="accent1"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1026,27 +1057,27 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
@@ -1309,10 +1340,10 @@
         <a:noFill/>
         <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1609,7 +1640,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1897,641 +1928,658 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IV34"/>
+  <dimension ref="A1:IT43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B31" sqref="B31:F31"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="20.100000000000001" customHeight="1" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="256" width="16.33203125" style="1" customWidth="1"/>
+    <col min="1" max="5" width="16.28515625" style="1" customWidth="1"/>
+    <col min="6" max="8" width="16.28515625" style="1" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="254" width="16.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:8" ht="27.6" customHeight="1">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-    </row>
-    <row r="2" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+    </row>
+    <row r="2" spans="1:8" ht="20.25" customHeight="1">
+      <c r="A2" s="4"/>
+      <c r="B2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" ht="24.2" customHeight="1">
+      <c r="A3" s="7"/>
+      <c r="B3" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+    </row>
+    <row r="4" spans="1:8" ht="21.6" customHeight="1">
+      <c r="A4" s="8"/>
+      <c r="B4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="20.85" customHeight="1">
+      <c r="A5" s="8"/>
+      <c r="B5" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="20.85" customHeight="1">
+      <c r="A6" s="8"/>
+      <c r="B6" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="20.85" customHeight="1">
+      <c r="A7" s="8"/>
+      <c r="B7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="20.85" customHeight="1">
+      <c r="A8" s="8"/>
+      <c r="B8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="20.85" customHeight="1">
+      <c r="A9" s="8"/>
+      <c r="B9" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="20.85" customHeight="1">
+      <c r="A10" s="8"/>
+      <c r="B10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="20.85" customHeight="1">
+      <c r="A11" s="8"/>
+      <c r="B11" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="20.85" customHeight="1">
+      <c r="A12" s="8"/>
+      <c r="B12" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="20.85" customHeight="1">
+      <c r="A13" s="8"/>
+      <c r="B13" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="20.85" customHeight="1">
+      <c r="A14" s="8"/>
+      <c r="B14" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="20.85" customHeight="1">
+      <c r="A15" s="8"/>
+      <c r="B15" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="20.85" customHeight="1">
+      <c r="A16" s="8"/>
+      <c r="B16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="20.85" customHeight="1">
+      <c r="A17" s="8"/>
+      <c r="B17" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="20.85" customHeight="1">
+      <c r="A18" s="8"/>
+      <c r="B18" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="20.85" customHeight="1">
+      <c r="A19" s="8"/>
+      <c r="B19" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="20.85" customHeight="1">
+      <c r="A20" s="8"/>
+      <c r="B20" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="20.85" customHeight="1">
+      <c r="A21" s="8"/>
+      <c r="B21" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="20.85" customHeight="1">
+      <c r="A22" s="8"/>
+      <c r="B22" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="20.85" customHeight="1">
+      <c r="A23" s="8"/>
+      <c r="B23" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="20.85" customHeight="1">
+      <c r="A24" s="8"/>
+      <c r="B24" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="24.6" customHeight="1">
+      <c r="A25" s="8"/>
+      <c r="B25" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="20.85" customHeight="1">
+      <c r="A26" s="8"/>
+      <c r="B26" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" ht="24.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="3"/>
-      <c r="B3" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-    </row>
-    <row r="4" spans="1:7" ht="21.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="4"/>
-      <c r="B5" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D5" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="4"/>
-      <c r="B6" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="4"/>
-      <c r="B7" s="8" t="s">
+      <c r="C26" s="23"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="19"/>
+      <c r="H26" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G7" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="4"/>
-      <c r="B8" s="8" t="s">
+    </row>
+    <row r="27" spans="1:8" ht="20.85" customHeight="1">
+      <c r="A27" s="8"/>
+      <c r="B27" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="19"/>
+      <c r="H27" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D8" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G8" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="4"/>
-      <c r="B9" s="8" t="s">
+    </row>
+    <row r="28" spans="1:8" ht="20.85" customHeight="1">
+      <c r="A28" s="8"/>
+      <c r="B28" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="23"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="15"/>
+      <c r="H28" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G9" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="4"/>
-      <c r="B10" s="8" t="s">
+    </row>
+    <row r="29" spans="1:8" ht="32.1" customHeight="1">
+      <c r="A29" s="8"/>
+      <c r="B29" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="23"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="19"/>
+      <c r="H29" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G10" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="4"/>
-      <c r="B11" s="8" t="s">
+    </row>
+    <row r="30" spans="1:8" ht="30.95" customHeight="1">
+      <c r="A30" s="8"/>
+      <c r="B30" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="23"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="19"/>
+      <c r="H30" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G11" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="4"/>
-      <c r="B12" s="8" t="s">
+    </row>
+    <row r="31" spans="1:8" ht="23.1" customHeight="1">
+      <c r="A31" s="8"/>
+      <c r="B31" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="15"/>
+      <c r="H31" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="4"/>
-      <c r="B13" s="8" t="s">
+    </row>
+    <row r="32" spans="1:8" ht="23.1" customHeight="1">
+      <c r="A32" s="8"/>
+      <c r="B32" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="23"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="H32" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D13" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G13" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="4"/>
-      <c r="B14" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D14" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G14" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="4"/>
-      <c r="B15" s="8" t="s">
+    </row>
+    <row r="33" spans="1:8" ht="18" customHeight="1">
+      <c r="A33" s="8"/>
+      <c r="B33" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="23"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="H33" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D15" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G15" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="4"/>
-      <c r="B16" s="8" t="s">
+    </row>
+    <row r="34" spans="1:8" ht="32.85" customHeight="1">
+      <c r="A34" s="8"/>
+      <c r="B34" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="23"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="19"/>
+      <c r="H34" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D16" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G16" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="4"/>
-      <c r="B17" s="8" t="s">
+    </row>
+    <row r="35" spans="1:8" ht="20.100000000000001" customHeight="1">
+      <c r="H35" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D17" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G17" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="4"/>
-      <c r="B18" s="8" t="s">
+    </row>
+    <row r="36" spans="1:8" ht="20.100000000000001" customHeight="1">
+      <c r="H36" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D18" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G18" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="4"/>
-      <c r="B19" s="8" t="s">
+    </row>
+    <row r="37" spans="1:8" ht="20.100000000000001" customHeight="1">
+      <c r="H37" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G19" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="4"/>
-      <c r="B20" s="8" t="s">
+    </row>
+    <row r="38" spans="1:8" ht="20.100000000000001" customHeight="1">
+      <c r="H38" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D20" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F20" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G20" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="4"/>
-      <c r="B21" s="8" t="s">
+    </row>
+    <row r="39" spans="1:8" ht="20.100000000000001" customHeight="1">
+      <c r="H39" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D21" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F21" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G21" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="4"/>
-      <c r="B22" s="8" t="s">
+    </row>
+    <row r="40" spans="1:8" ht="20.100000000000001" customHeight="1">
+      <c r="H40" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D22" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F22" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G22" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="4"/>
-      <c r="B23" s="8" t="s">
+    </row>
+    <row r="41" spans="1:8" ht="20.100000000000001" customHeight="1">
+      <c r="H41" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D23" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F23" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G23" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="4"/>
-      <c r="B24" s="8" t="s">
+    </row>
+    <row r="42" spans="1:8" ht="20.100000000000001" customHeight="1">
+      <c r="H42" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D24" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F24" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G24" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="24.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="4"/>
-      <c r="B25" s="14" t="s">
+    </row>
+    <row r="43" spans="1:8" ht="20.100000000000001" customHeight="1">
+      <c r="H43" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="17"/>
-    </row>
-    <row r="26" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="18"/>
-      <c r="B26" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="18"/>
-      <c r="B27" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="22" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="18"/>
-      <c r="B28" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="18"/>
-      <c r="B29" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="22" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="18"/>
-      <c r="B30" s="19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="32.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="18"/>
-      <c r="B31" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="22" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="18"/>
-      <c r="B32" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="29" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="18"/>
-      <c r="B33" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="28"/>
-      <c r="G33" s="30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="18"/>
-      <c r="B34" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="30" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B34:D34"/>
   </mergeCells>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C24 E5:E24" xr:uid="{57F07D11-7A0D-8942-94C6-F3B3B20B2CAC}">
+      <formula1>$F$5:$F$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E28" xr:uid="{0160D12D-E8D8-7A4D-BB71-013E88A81347}">
+      <formula1>$G$9:$G$11</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E31" xr:uid="{04288AD5-A2CC-404A-A02C-F6975BC8B309}">
+      <formula1>$G$4:$G$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E32:E33" xr:uid="{1FAC0C7C-2A07-2449-B288-4E800EF34002}">
+      <formula1>$G$7:$G$8</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E26:E27 E29:E30 E34" xr:uid="{A8E702C3-7B84-9C49-B473-1782733E72A4}">
+      <formula1>$H$3:$H$43</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>